<commit_message>
More info regarding data in two file formats again
</commit_message>
<xml_diff>
--- a/proj.xlsx
+++ b/proj.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
   <si>
     <t>height</t>
   </si>
@@ -41,15 +41,37 @@
   <si>
     <t>difference between calculated and actual</t>
   </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +94,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="45">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96:C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -479,15 +589,15 @@
         <v>102.75</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">(C3*COS((PI()*B3/180))/-9.8)*(-C3*SIN(PI()*B3/180)-SQRT((C3*SIN(PI()*B3/180))^2-2*(-9.8)*(0.91+0.003*B3)))*100</f>
+        <f t="shared" ref="E3:E16" si="0">(C3*COS((PI()*B3/180))/-9.8)*(-C3*SIN(PI()*B3/180)-SQRT((C3*SIN(PI()*B3/180))^2-2*(-9.8)*(0.91+0.003*B3)))*100</f>
         <v>120.66482503198684</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="1">E3-D3</f>
+        <f t="shared" ref="F3:F16" si="1">E3-D3</f>
         <v>17.914825031986837</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="2">(E3/D3-1)*100</f>
+        <f t="shared" ref="G3:G16" si="2">(E3/D3-1)*100</f>
         <v>17.435352829184268</v>
       </c>
     </row>
@@ -830,1147 +940,976 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17">
-        <v>55</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
+      <c r="B17" t="s">
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>2.6429999999999998</v>
+        <f>AVERAGE(C2:C16)</f>
+        <v>3.0437333333333338</v>
       </c>
       <c r="D17">
-        <v>102.26</v>
+        <f>AVERAGE(D2:D16)</f>
+        <v>111.24666666666666</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>126.84197811398077</v>
+        <f t="shared" ref="E17:G17" si="3">AVERAGE(E2:E16)</f>
+        <v>131.16841075381885</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
-        <v>24.581978113980767</v>
+        <f t="shared" si="3"/>
+        <v>19.921744087152167</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
-        <v>24.038703416761955</v>
+        <f t="shared" si="3"/>
+        <v>17.93213822060374</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18">
-        <v>55</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
+      <c r="B18" t="s">
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>2.6520000000000001</v>
+        <f>STDEV(C2:C16)</f>
+        <v>0.19464967310040684</v>
       </c>
       <c r="D18">
-        <v>102.68</v>
+        <f>STDEV(D2:D16)</f>
+        <v>6.7923472343793598</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>127.31998836756769</v>
+        <f>STDEV(E2:E16)</f>
+        <v>8.3883459811407217</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>24.639988367567682</v>
+        <f>STDEV(F2:F16)</f>
+        <v>3.8080849887815895</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
-        <v>23.996872192800623</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>55</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>2.6429999999999998</v>
-      </c>
-      <c r="D19">
-        <v>103.22</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>126.84197811398077</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>23.621978113980774</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="2"/>
-        <v>22.885078583589191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>60</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20">
-        <v>2.7170000000000001</v>
-      </c>
-      <c r="D20">
-        <v>107.63</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>130.78202530812263</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>23.152025308122631</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="2"/>
-        <v>21.510754722774905</v>
+        <f>STDEV(G2:G16)</f>
+        <v>3.2844849943090382</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21">
-        <v>60</v>
-      </c>
-      <c r="B21">
-        <v>10</v>
-      </c>
-      <c r="C21">
-        <v>2.7309999999999999</v>
-      </c>
-      <c r="D21">
-        <v>107.64</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>131.52993788445073</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>23.889937884450731</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>22.194293835424304</v>
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>2.7360000000000002</v>
+        <v>2.6429999999999998</v>
       </c>
       <c r="D22">
-        <v>107.02</v>
+        <v>102.26</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>131.79724246198808</v>
+        <f t="shared" ref="E22:E36" si="4">(C22*COS((PI()*B22/180))/-9.8)*(-C22*SIN(PI()*B22/180)-SQRT((C22*SIN(PI()*B22/180))^2-2*(-9.8)*(0.91+0.003*B22)))*100</f>
+        <v>126.84197811398077</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
-        <v>24.777242461988081</v>
+        <f t="shared" ref="F22:F36" si="5">E22-D22</f>
+        <v>24.581978113980767</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
-        <v>23.151973894588007</v>
+        <f t="shared" ref="G22:G36" si="6">(E22/D22-1)*100</f>
+        <v>24.038703416761955</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23">
-        <v>2.8690000000000002</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="D23">
-        <v>114.47</v>
+        <v>102.68</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>138.94491630057121</v>
+        <f t="shared" si="4"/>
+        <v>127.31998836756769</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
-        <v>24.474916300571209</v>
+        <f t="shared" si="5"/>
+        <v>24.639988367567682</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
-        <v>21.381074779917199</v>
+        <f t="shared" si="6"/>
+        <v>23.996872192800623</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
       <c r="C24">
-        <v>2.8980000000000001</v>
+        <v>2.6429999999999998</v>
       </c>
       <c r="D24">
-        <v>115.29</v>
+        <v>103.22</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>140.51302444888836</v>
+        <f t="shared" si="4"/>
+        <v>126.84197811398077</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
-        <v>25.223024448888353</v>
+        <f t="shared" si="5"/>
+        <v>23.621978113980774</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
-        <v>21.877894395774433</v>
+        <f t="shared" si="6"/>
+        <v>22.885078583589191</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>2.8879999999999999</v>
+        <v>2.7170000000000001</v>
       </c>
       <c r="D25">
-        <v>113.56</v>
+        <v>107.63</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>139.97190855572543</v>
+        <f t="shared" si="4"/>
+        <v>130.78202530812263</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
-        <v>26.411908555725432</v>
+        <f t="shared" si="5"/>
+        <v>23.152025308122631</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
-        <v>23.258108978271785</v>
+        <f t="shared" si="6"/>
+        <v>21.510754722774905</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26">
-        <v>3.1179999999999999</v>
+        <v>2.7309999999999999</v>
       </c>
       <c r="D26">
-        <v>101.58</v>
+        <v>107.64</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>152.52158576145948</v>
+        <f t="shared" si="4"/>
+        <v>131.52993788445073</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>50.941585761459478</v>
+        <f t="shared" si="5"/>
+        <v>23.889937884450731</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
-        <v>50.149227959696276</v>
+        <f t="shared" si="6"/>
+        <v>22.194293835424304</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>10</v>
       </c>
       <c r="C27">
-        <v>2.9489999999999998</v>
+        <v>2.7360000000000002</v>
       </c>
       <c r="D27">
-        <v>118.02</v>
+        <v>107.02</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>143.27909246375526</v>
+        <f t="shared" si="4"/>
+        <v>131.79724246198808</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
-        <v>25.259092463755266</v>
+        <f t="shared" si="5"/>
+        <v>24.777242461988081</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
-        <v>21.402383039955318</v>
+        <f t="shared" si="6"/>
+        <v>23.151973894588007</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28">
-        <v>2.9470000000000001</v>
+        <v>2.8690000000000002</v>
       </c>
       <c r="D28">
-        <v>118.81</v>
+        <v>114.47</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>143.17041812972639</v>
+        <f t="shared" si="4"/>
+        <v>138.94491630057121</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
-        <v>24.360418129726384</v>
+        <f t="shared" si="5"/>
+        <v>24.474916300571209</v>
       </c>
       <c r="G28">
-        <f t="shared" si="2"/>
-        <v>20.503676567398688</v>
+        <f t="shared" si="6"/>
+        <v>21.381074779917199</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29">
-        <v>3.1059999999999999</v>
+        <v>2.8980000000000001</v>
       </c>
       <c r="D29">
-        <v>119.68</v>
+        <v>115.29</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>151.86142411669636</v>
+        <f t="shared" si="4"/>
+        <v>140.51302444888836</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
-        <v>32.181424116696348</v>
+        <f t="shared" si="5"/>
+        <v>25.223024448888353</v>
       </c>
       <c r="G29">
-        <f t="shared" si="2"/>
-        <v>26.889558921036393</v>
+        <f t="shared" si="6"/>
+        <v>21.877894395774433</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
       <c r="C30">
-        <v>3.2480000000000002</v>
+        <v>2.8879999999999999</v>
       </c>
       <c r="D30">
-        <v>125.42</v>
+        <v>113.56</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>159.71163897801529</v>
+        <f t="shared" si="4"/>
+        <v>139.97190855572543</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
-        <v>34.291638978015285</v>
+        <f t="shared" si="5"/>
+        <v>26.411908555725432</v>
       </c>
       <c r="G30">
-        <f t="shared" si="2"/>
-        <v>27.341443930804733</v>
+        <f t="shared" si="6"/>
+        <v>23.258108978271785</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B31">
         <v>10</v>
       </c>
       <c r="C31">
-        <v>3.3029999999999999</v>
+        <v>3.1179999999999999</v>
       </c>
       <c r="D31">
-        <v>128.27000000000001</v>
+        <v>101.58</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>162.77476423635625</v>
+        <f t="shared" si="4"/>
+        <v>152.52158576145948</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
-        <v>34.504764236356237</v>
+        <f t="shared" si="5"/>
+        <v>50.941585761459478</v>
       </c>
       <c r="G31">
-        <f t="shared" si="2"/>
-        <v>26.900104651404245</v>
+        <f t="shared" si="6"/>
+        <v>50.149227959696276</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>2.4990000000000001</v>
+        <v>2.9489999999999998</v>
       </c>
       <c r="D32">
-        <v>96.27</v>
+        <v>118.02</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>126.95068547919706</v>
+        <f t="shared" si="4"/>
+        <v>143.27909246375526</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
-        <v>30.680685479197066</v>
+        <f t="shared" si="5"/>
+        <v>25.259092463755266</v>
       </c>
       <c r="G32">
-        <f t="shared" si="2"/>
-        <v>31.869414645473213</v>
+        <f t="shared" si="6"/>
+        <v>21.402383039955318</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>2.4689999999999999</v>
+        <v>2.9470000000000001</v>
       </c>
       <c r="D33">
-        <v>95.36</v>
+        <v>118.81</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
-        <v>125.13729591500721</v>
+        <f t="shared" si="4"/>
+        <v>143.17041812972639</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
-        <v>29.777295915007215</v>
+        <f t="shared" si="5"/>
+        <v>24.360418129726384</v>
       </c>
       <c r="G33">
-        <f t="shared" si="2"/>
-        <v>31.226191186039443</v>
+        <f t="shared" si="6"/>
+        <v>20.503676567398688</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C34">
-        <v>2.6520000000000001</v>
+        <v>3.1059999999999999</v>
       </c>
       <c r="D34">
-        <v>114.14</v>
+        <v>119.68</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
-        <v>136.31736576282532</v>
+        <f t="shared" si="4"/>
+        <v>151.86142411669636</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
-        <v>22.177365762825318</v>
+        <f t="shared" si="5"/>
+        <v>32.181424116696348</v>
       </c>
       <c r="G34">
-        <f t="shared" si="2"/>
-        <v>19.429968251993436</v>
+        <f t="shared" si="6"/>
+        <v>26.889558921036393</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C35">
-        <v>2.5819999999999999</v>
+        <v>3.2480000000000002</v>
       </c>
       <c r="D35">
-        <v>112.43</v>
+        <v>125.42</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>132.0073124001625</v>
+        <f t="shared" si="4"/>
+        <v>159.71163897801529</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
-        <v>19.577312400162498</v>
+        <f t="shared" si="5"/>
+        <v>34.291638978015285</v>
       </c>
       <c r="G35">
-        <f t="shared" si="2"/>
-        <v>17.412890154018058</v>
+        <f t="shared" si="6"/>
+        <v>27.341443930804733</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C36">
-        <v>2.6339999999999999</v>
+        <v>3.3029999999999999</v>
       </c>
       <c r="D36">
-        <v>105.6</v>
+        <v>128.27000000000001</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
-        <v>135.20508143909518</v>
+        <f t="shared" si="4"/>
+        <v>162.77476423635625</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
-        <v>29.605081439095187</v>
+        <f t="shared" si="5"/>
+        <v>34.504764236356237</v>
       </c>
       <c r="G36">
-        <f t="shared" si="2"/>
-        <v>28.035114999143175</v>
+        <f t="shared" si="6"/>
+        <v>26.900104651404245</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37">
-        <v>65</v>
-      </c>
-      <c r="B37">
-        <v>20</v>
+      <c r="B37" t="s">
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>2.7650000000000001</v>
+        <f>AVERAGE(C22:C36)</f>
+        <v>2.8965333333333332</v>
       </c>
       <c r="D37">
-        <v>110.71</v>
+        <f>AVERAGE(D22:D36)</f>
+        <v>112.36999999999999</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
-        <v>143.36337451395528</v>
+        <f t="shared" ref="E37" si="7">AVERAGE(E22:E36)</f>
+        <v>140.52412821608561</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
-        <v>32.653374513955285</v>
+        <f t="shared" ref="F37" si="8">AVERAGE(F22:F36)</f>
+        <v>28.154128216085649</v>
       </c>
       <c r="G37">
-        <f t="shared" si="2"/>
-        <v>29.49451225178872</v>
+        <f t="shared" ref="G37" si="9">AVERAGE(G22:G36)</f>
+        <v>25.165409991346543</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38">
-        <v>65</v>
-      </c>
-      <c r="B38">
-        <v>20</v>
+      <c r="B38" t="s">
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>2.7850000000000001</v>
+        <f>STDEV(C22:C36)</f>
+        <v>0.21738046523702784</v>
       </c>
       <c r="D38">
-        <v>110.889</v>
+        <f>STDEV(D22:D36)</f>
+        <v>8.5940801884619571</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
-        <v>144.62188283564313</v>
+        <f>STDEV(E22:E36)</f>
+        <v>11.813523221289227</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
-        <v>33.732882835643139</v>
+        <f>STDEV(F22:F36)</f>
+        <v>7.3760289689466232</v>
       </c>
       <c r="G38">
-        <f t="shared" si="2"/>
-        <v>30.420404941556999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39">
-        <v>65</v>
-      </c>
-      <c r="B39">
-        <v>20</v>
-      </c>
-      <c r="C39">
-        <v>2.8050000000000002</v>
-      </c>
-      <c r="D39">
-        <v>109.8</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>145.88384193653715</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="1"/>
-        <v>36.083841936537155</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="2"/>
-        <v>32.863244022347125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40">
-        <v>70</v>
-      </c>
-      <c r="B40">
-        <v>20</v>
-      </c>
-      <c r="C40">
-        <v>2.92</v>
-      </c>
-      <c r="D40">
-        <v>118.22</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>153.20734815036445</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
-        <v>34.987348150364454</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="2"/>
-        <v>29.595117704588446</v>
+        <f>STDEV(G22:G36)</f>
+        <v>7.2389809821966464</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41">
-        <v>70</v>
-      </c>
-      <c r="B41">
-        <v>20</v>
-      </c>
-      <c r="C41">
-        <v>2.9089999999999998</v>
-      </c>
-      <c r="D41">
-        <v>118.63</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>152.50186785895028</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="1"/>
-        <v>33.871867858950282</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="2"/>
-        <v>28.552531281252879</v>
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B42">
         <v>20</v>
       </c>
       <c r="C42">
-        <v>2.931</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="D42">
-        <v>117.91</v>
+        <v>96.27</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
-        <v>153.91388345954533</v>
+        <f t="shared" ref="E42:E55" si="10">(C42*COS((PI()*B42/180))/-9.8)*(-C42*SIN(PI()*B42/180)-SQRT((C42*SIN(PI()*B42/180))^2-2*(-9.8)*(0.91+0.003*B42)))*100</f>
+        <v>126.95068547919706</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
-        <v>36.003883459545335</v>
+        <f t="shared" ref="F42:F55" si="11">E42-D42</f>
+        <v>30.680685479197066</v>
       </c>
       <c r="G42">
-        <f t="shared" si="2"/>
-        <v>30.535055092481844</v>
+        <f t="shared" ref="G42:G55" si="12">(E42/D42-1)*100</f>
+        <v>31.869414645473213</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>20</v>
       </c>
       <c r="C43">
-        <v>2.9980000000000002</v>
+        <v>2.4689999999999999</v>
       </c>
       <c r="D43">
-        <v>125.01</v>
+        <v>95.36</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
-        <v>158.24016150733169</v>
+        <f t="shared" si="10"/>
+        <v>125.13729591500721</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
-        <v>33.230161507331687</v>
+        <f t="shared" si="11"/>
+        <v>29.777295915007215</v>
       </c>
       <c r="G43">
-        <f t="shared" si="2"/>
-        <v>26.582002645653692</v>
+        <f t="shared" si="12"/>
+        <v>31.226191186039443</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B44">
         <v>20</v>
       </c>
       <c r="C44">
-        <v>2.9870000000000001</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="D44">
-        <v>123.36</v>
+        <v>114.14</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
-        <v>157.52718070095327</v>
+        <f t="shared" si="10"/>
+        <v>136.31736576282532</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
-        <v>34.167180700953267</v>
+        <f t="shared" si="11"/>
+        <v>22.177365762825318</v>
       </c>
       <c r="G44">
-        <f t="shared" si="2"/>
-        <v>27.697130918412171</v>
+        <f t="shared" si="12"/>
+        <v>19.429968251993436</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B45">
         <v>20</v>
       </c>
       <c r="C45">
-        <v>2.964</v>
+        <v>2.5819999999999999</v>
       </c>
       <c r="D45">
-        <v>120.56</v>
+        <v>112.43</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
-        <v>156.03982852444423</v>
+        <f t="shared" si="10"/>
+        <v>132.0073124001625</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
-        <v>35.47982852444423</v>
+        <f t="shared" si="11"/>
+        <v>19.577312400162498</v>
       </c>
       <c r="G45">
-        <f t="shared" si="2"/>
-        <v>29.429187561748705</v>
+        <f t="shared" si="12"/>
+        <v>17.412890154018058</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B46">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C46">
-        <v>2.3010000000000002</v>
+        <v>2.6339999999999999</v>
       </c>
       <c r="D46">
-        <v>89.38</v>
+        <v>105.6</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
-        <v>116.40637495740059</v>
+        <f t="shared" si="10"/>
+        <v>135.20508143909518</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
-        <v>27.026374957400591</v>
+        <f t="shared" si="11"/>
+        <v>29.605081439095187</v>
       </c>
       <c r="G46">
-        <f t="shared" si="2"/>
-        <v>30.237609037145429</v>
+        <f t="shared" si="12"/>
+        <v>28.035114999143175</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B47">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C47">
-        <v>2.2480000000000002</v>
+        <v>2.7650000000000001</v>
       </c>
       <c r="D47">
-        <v>89.77</v>
+        <v>110.71</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
-        <v>113.06771793284804</v>
+        <f t="shared" si="10"/>
+        <v>143.36337451395528</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
-        <v>23.297717932848045</v>
+        <f t="shared" si="11"/>
+        <v>32.653374513955285</v>
       </c>
       <c r="G47">
-        <f t="shared" si="2"/>
-        <v>25.952676766010963</v>
+        <f t="shared" si="12"/>
+        <v>29.49451225178872</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B48">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>2.2029999999999998</v>
+        <v>2.7850000000000001</v>
       </c>
       <c r="D48">
-        <v>88.18</v>
+        <v>110.889</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
-        <v>110.2595494589352</v>
+        <f t="shared" si="10"/>
+        <v>144.62188283564313</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
-        <v>22.07954945893519</v>
+        <f t="shared" si="11"/>
+        <v>33.732882835643139</v>
       </c>
       <c r="G48">
-        <f t="shared" si="2"/>
-        <v>25.039180606640031</v>
+        <f t="shared" si="12"/>
+        <v>30.420404941556999</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B49">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C49">
-        <v>2.4369999999999998</v>
+        <v>2.8050000000000002</v>
       </c>
       <c r="D49">
-        <v>98.52</v>
+        <v>109.8</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
-        <v>125.12946217619303</v>
+        <f t="shared" si="10"/>
+        <v>145.88384193653715</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
-        <v>26.609462176193034</v>
+        <f t="shared" si="11"/>
+        <v>36.083841936537155</v>
       </c>
       <c r="G49">
-        <f t="shared" si="2"/>
-        <v>27.009198311198766</v>
+        <f t="shared" si="12"/>
+        <v>32.863244022347125</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B50">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C50">
-        <v>2.3559999999999999</v>
+        <v>2.92</v>
       </c>
       <c r="D50">
-        <v>98.18</v>
+        <v>118.22</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
-        <v>119.90696043754765</v>
+        <f t="shared" si="10"/>
+        <v>153.20734815036445</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
-        <v>21.726960437547646</v>
+        <f t="shared" si="11"/>
+        <v>34.987348150364454</v>
       </c>
       <c r="G50">
-        <f t="shared" si="2"/>
-        <v>22.129721366416423</v>
+        <f t="shared" si="12"/>
+        <v>29.595117704588446</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B51">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C51">
-        <v>2.3420000000000001</v>
+        <v>2.9089999999999998</v>
       </c>
       <c r="D51">
-        <v>93.32</v>
+        <v>118.63</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
-        <v>119.01241777398195</v>
+        <f t="shared" si="10"/>
+        <v>152.50186785895028</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
-        <v>25.692417773981958</v>
+        <f t="shared" si="11"/>
+        <v>33.871867858950282</v>
       </c>
       <c r="G51">
-        <f t="shared" si="2"/>
-        <v>27.531523546915949</v>
+        <f t="shared" si="12"/>
+        <v>28.552531281252879</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B52">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <v>2.508</v>
+        <v>2.931</v>
       </c>
       <c r="D52">
-        <v>116.68</v>
+        <v>117.91</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
-        <v>129.77340716687695</v>
+        <f t="shared" si="10"/>
+        <v>153.91388345954533</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
-        <v>13.093407166876943</v>
+        <f t="shared" si="11"/>
+        <v>36.003883459545335</v>
       </c>
       <c r="G52">
-        <f t="shared" si="2"/>
-        <v>11.221637955842434</v>
+        <f t="shared" si="12"/>
+        <v>30.535055092481844</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B53">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>2.5</v>
+        <v>2.9980000000000002</v>
       </c>
       <c r="D53">
-        <v>114.69</v>
+        <v>125.01</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
-        <v>129.24703923924841</v>
+        <f t="shared" si="10"/>
+        <v>158.24016150733169</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
-        <v>14.557039239248411</v>
+        <f t="shared" si="11"/>
+        <v>33.230161507331687</v>
       </c>
       <c r="G53">
-        <f t="shared" si="2"/>
-        <v>12.692509581697099</v>
+        <f t="shared" si="12"/>
+        <v>26.582002645653692</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B54">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>2.524</v>
+        <v>2.9870000000000001</v>
       </c>
       <c r="D54">
-        <v>117.98</v>
+        <v>123.36</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
-        <v>130.82851678366566</v>
+        <f t="shared" si="10"/>
+        <v>157.52718070095327</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
-        <v>12.848516783665659</v>
+        <f t="shared" si="11"/>
+        <v>34.167180700953267</v>
       </c>
       <c r="G54">
-        <f t="shared" si="2"/>
-        <v>10.890419379272466</v>
+        <f t="shared" si="12"/>
+        <v>27.697130918412171</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B55">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>2.6520000000000001</v>
+        <v>2.964</v>
       </c>
       <c r="D55">
-        <v>110.41</v>
+        <v>120.56</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
-        <v>139.38390739435351</v>
+        <f t="shared" si="10"/>
+        <v>156.03982852444423</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
-        <v>28.973907394353517</v>
+        <f t="shared" si="11"/>
+        <v>35.47982852444423</v>
       </c>
       <c r="G55">
-        <f t="shared" si="2"/>
-        <v>26.24210433326104</v>
+        <f t="shared" si="12"/>
+        <v>29.429187561748705</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56">
-        <v>70</v>
-      </c>
-      <c r="B56">
-        <v>30</v>
+      <c r="B56" t="s">
+        <v>8</v>
       </c>
       <c r="C56">
-        <v>2.661</v>
+        <f>AVERAGE(C42:C55)</f>
+        <v>2.7785714285714289</v>
       </c>
       <c r="D56">
-        <v>112.19</v>
+        <f>AVERAGE(D42:D55)</f>
+        <v>112.77778571428571</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
-        <v>139.99315699248268</v>
+        <f t="shared" ref="E56:G56" si="13">AVERAGE(E42:E55)</f>
+        <v>144.35122217742943</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
-        <v>27.803156992482684</v>
+        <f t="shared" si="13"/>
+        <v>31.573436463143725</v>
       </c>
       <c r="G56">
-        <f t="shared" si="2"/>
-        <v>24.78220607227264</v>
+        <f t="shared" si="13"/>
+        <v>28.081626118321278</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57">
-        <v>70</v>
-      </c>
-      <c r="B57">
-        <v>30</v>
+      <c r="B57" t="s">
+        <v>7</v>
       </c>
       <c r="C57">
-        <v>2.67</v>
+        <f>STDEV(C42:C55)</f>
+        <v>0.18328276358831846</v>
       </c>
       <c r="D57">
-        <v>114.98</v>
+        <f>STDEV(D42:D55)</f>
+        <v>9.0233577766779316</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
-        <v>140.60342287745806</v>
+        <f>STDEV(E42:E55)</f>
+        <v>11.486979355718505</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
-        <v>25.623422877458054</v>
+        <f>STDEV(F42:F55)</f>
+        <v>5.0196728567118161</v>
       </c>
       <c r="G57">
-        <f t="shared" si="2"/>
-        <v>22.285112956564657</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58">
-        <v>75</v>
-      </c>
-      <c r="B58">
-        <v>30</v>
-      </c>
-      <c r="C58">
-        <v>2.78</v>
-      </c>
-      <c r="D58">
-        <v>120</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="0"/>
-        <v>148.14468184498614</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="1"/>
-        <v>28.144681844986138</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="2"/>
-        <v>23.453901537488452</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59">
-        <v>75</v>
-      </c>
-      <c r="B59">
-        <v>30</v>
-      </c>
-      <c r="C59">
-        <v>2.82</v>
-      </c>
-      <c r="D59">
-        <v>120.83</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="0"/>
-        <v>150.9249413420371</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="1"/>
-        <v>30.094941342037103</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="2"/>
-        <v>24.906845437422078</v>
+        <f>STDEV(G42:G55)</f>
+        <v>4.4374738146641013</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60">
-        <v>75</v>
-      </c>
-      <c r="B60">
-        <v>30</v>
-      </c>
-      <c r="C60">
-        <v>2.7949999999999999</v>
-      </c>
-      <c r="D60">
-        <v>122.34</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="0"/>
-        <v>149.18489592068534</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="1"/>
-        <v>26.844895920685332</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="2"/>
-        <v>21.942860814684749</v>
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1978,25 +1917,25 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C61">
-        <v>2.1549999999999998</v>
+        <v>2.3010000000000002</v>
       </c>
       <c r="D61">
-        <v>72.040000000000006</v>
+        <v>89.38</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
-        <v>102.53639567585282</v>
+        <f t="shared" ref="E61:E75" si="14">(C61*COS((PI()*B61/180))/-9.8)*(-C61*SIN(PI()*B61/180)-SQRT((C61*SIN(PI()*B61/180))^2-2*(-9.8)*(0.91+0.003*B61)))*100</f>
+        <v>116.40637495740059</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
-        <v>30.49639567585281</v>
+        <f t="shared" ref="F61:F75" si="15">E61-D61</f>
+        <v>27.026374957400591</v>
       </c>
       <c r="G61">
-        <f t="shared" si="2"/>
-        <v>42.332587001461434</v>
+        <f t="shared" ref="G61:G75" si="16">(E61/D61-1)*100</f>
+        <v>30.237609037145429</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2004,25 +1943,25 @@
         <v>55</v>
       </c>
       <c r="B62">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C62">
-        <v>2.0859999999999999</v>
+        <v>2.2480000000000002</v>
       </c>
       <c r="D62">
-        <v>68.98</v>
+        <v>89.77</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
-        <v>98.320186470314496</v>
+        <f t="shared" si="14"/>
+        <v>113.06771793284804</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
-        <v>29.340186470314492</v>
+        <f t="shared" si="15"/>
+        <v>23.297717932848045</v>
       </c>
       <c r="G62">
-        <f t="shared" si="2"/>
-        <v>42.534338170940124</v>
+        <f t="shared" si="16"/>
+        <v>25.952676766010963</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2030,25 +1969,25 @@
         <v>55</v>
       </c>
       <c r="B63">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C63">
-        <v>2.1429999999999998</v>
+        <v>2.2029999999999998</v>
       </c>
       <c r="D63">
-        <v>71.11</v>
+        <v>88.18</v>
       </c>
       <c r="E63">
-        <f t="shared" si="0"/>
-        <v>101.79824621087627</v>
+        <f t="shared" si="14"/>
+        <v>110.2595494589352</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
-        <v>30.688246210876272</v>
+        <f t="shared" si="15"/>
+        <v>22.07954945893519</v>
       </c>
       <c r="G63">
-        <f t="shared" si="2"/>
-        <v>43.156020546865804</v>
+        <f t="shared" si="16"/>
+        <v>25.039180606640031</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2056,25 +1995,25 @@
         <v>60</v>
       </c>
       <c r="B64">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C64">
-        <v>2.2509999999999999</v>
+        <v>2.4369999999999998</v>
       </c>
       <c r="D64">
-        <v>80.540000000000006</v>
+        <v>98.52</v>
       </c>
       <c r="E64">
-        <f t="shared" si="0"/>
-        <v>108.51628936054276</v>
+        <f t="shared" si="14"/>
+        <v>125.12946217619303</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
-        <v>27.976289360542751</v>
+        <f t="shared" si="15"/>
+        <v>26.609462176193034</v>
       </c>
       <c r="G64">
-        <f t="shared" si="2"/>
-        <v>34.735894413388067</v>
+        <f t="shared" si="16"/>
+        <v>27.009198311198766</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2082,25 +2021,25 @@
         <v>60</v>
       </c>
       <c r="B65">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C65">
-        <v>2.2250000000000001</v>
+        <v>2.3559999999999999</v>
       </c>
       <c r="D65">
-        <v>77.819999999999993</v>
+        <v>98.18</v>
       </c>
       <c r="E65">
-        <f t="shared" si="0"/>
-        <v>106.8835799183602</v>
+        <f t="shared" si="14"/>
+        <v>119.90696043754765</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
-        <v>29.063579918360205</v>
+        <f t="shared" si="15"/>
+        <v>21.726960437547646</v>
       </c>
       <c r="G65">
-        <f t="shared" si="2"/>
-        <v>37.347185708507084</v>
+        <f t="shared" si="16"/>
+        <v>22.129721366416423</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2108,25 +2047,25 @@
         <v>60</v>
       </c>
       <c r="B66">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C66">
-        <v>2.2610000000000001</v>
+        <v>2.3420000000000001</v>
       </c>
       <c r="D66">
-        <v>81.77</v>
+        <v>93.32</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
-        <v>109.14686737844946</v>
+        <f t="shared" si="14"/>
+        <v>119.01241777398195</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
-        <v>27.376867378449461</v>
+        <f t="shared" si="15"/>
+        <v>25.692417773981958</v>
       </c>
       <c r="G66">
-        <f t="shared" si="2"/>
-        <v>33.480331880212134</v>
+        <f t="shared" si="16"/>
+        <v>27.531523546915949</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2134,25 +2073,25 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C67">
-        <v>2.3809999999999998</v>
+        <v>2.508</v>
       </c>
       <c r="D67">
-        <v>86.65</v>
+        <v>116.68</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E75" si="3">(C67*COS((PI()*B67/180))/-9.8)*(-C67*SIN(PI()*B67/180)-SQRT((C67*SIN(PI()*B67/180))^2-2*(-9.8)*(0.91+0.003*B67)))*100</f>
-        <v>116.82770636493291</v>
+        <f t="shared" si="14"/>
+        <v>129.77340716687695</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F75" si="4">E67-D67</f>
-        <v>30.177706364932902</v>
+        <f t="shared" si="15"/>
+        <v>13.093407166876943</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G75" si="5">(E67/D67-1)*100</f>
-        <v>34.827127945681369</v>
+        <f t="shared" si="16"/>
+        <v>11.221637955842434</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2160,25 +2099,25 @@
         <v>65</v>
       </c>
       <c r="B68">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C68">
-        <v>2.415</v>
+        <v>2.5</v>
       </c>
       <c r="D68">
-        <v>89.38</v>
+        <v>114.69</v>
       </c>
       <c r="E68">
-        <f t="shared" si="3"/>
-        <v>119.04241182764423</v>
+        <f t="shared" si="14"/>
+        <v>129.24703923924841</v>
       </c>
       <c r="F68">
-        <f t="shared" si="4"/>
-        <v>29.662411827644235</v>
+        <f t="shared" si="15"/>
+        <v>14.557039239248411</v>
       </c>
       <c r="G68">
-        <f t="shared" si="5"/>
-        <v>33.186855927102535</v>
+        <f t="shared" si="16"/>
+        <v>12.692509581697099</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2186,25 +2125,25 @@
         <v>65</v>
       </c>
       <c r="B69">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C69">
-        <v>2.371</v>
+        <v>2.524</v>
       </c>
       <c r="D69">
-        <v>85.38</v>
+        <v>117.98</v>
       </c>
       <c r="E69">
-        <f t="shared" si="3"/>
-        <v>116.17956827878793</v>
+        <f t="shared" si="14"/>
+        <v>130.82851678366566</v>
       </c>
       <c r="F69">
-        <f t="shared" si="4"/>
-        <v>30.79956827878793</v>
+        <f t="shared" si="15"/>
+        <v>12.848516783665659</v>
       </c>
       <c r="G69">
-        <f t="shared" si="5"/>
-        <v>36.073516372438434</v>
+        <f t="shared" si="16"/>
+        <v>10.890419379272466</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2212,25 +2151,25 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C70">
-        <v>2.5529999999999999</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="D70">
-        <v>94.74</v>
+        <v>110.41</v>
       </c>
       <c r="E70">
-        <f t="shared" si="3"/>
-        <v>128.20777790883764</v>
+        <f t="shared" si="14"/>
+        <v>139.38390739435351</v>
       </c>
       <c r="F70">
-        <f t="shared" si="4"/>
-        <v>33.467777908837647</v>
+        <f t="shared" si="15"/>
+        <v>28.973907394353517</v>
       </c>
       <c r="G70">
-        <f t="shared" si="5"/>
-        <v>35.325921373060631</v>
+        <f t="shared" si="16"/>
+        <v>26.24210433326104</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2238,25 +2177,25 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C71">
-        <v>2.472</v>
+        <v>2.661</v>
       </c>
       <c r="D71">
-        <v>93.93</v>
+        <v>112.19</v>
       </c>
       <c r="E71">
-        <f t="shared" si="3"/>
-        <v>122.79370701846524</v>
+        <f t="shared" si="14"/>
+        <v>139.99315699248268</v>
       </c>
       <c r="F71">
-        <f t="shared" si="4"/>
-        <v>28.863707018465234</v>
+        <f t="shared" si="15"/>
+        <v>27.803156992482684</v>
       </c>
       <c r="G71">
-        <f t="shared" si="5"/>
-        <v>30.728954560273849</v>
+        <f t="shared" si="16"/>
+        <v>24.78220607227264</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2264,25 +2203,25 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C72">
-        <v>2.536</v>
+        <v>2.67</v>
       </c>
       <c r="D72">
-        <v>96.5</v>
+        <v>114.98</v>
       </c>
       <c r="E72">
-        <f t="shared" si="3"/>
-        <v>127.06335008836211</v>
+        <f t="shared" si="14"/>
+        <v>140.60342287745806</v>
       </c>
       <c r="F72">
-        <f t="shared" si="4"/>
-        <v>30.563350088362114</v>
+        <f t="shared" si="15"/>
+        <v>25.623422877458054</v>
       </c>
       <c r="G72">
-        <f t="shared" si="5"/>
-        <v>31.671865376541053</v>
+        <f t="shared" si="16"/>
+        <v>22.285112956564657</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2290,25 +2229,25 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C73">
-        <v>2.6539999999999999</v>
+        <v>2.78</v>
       </c>
       <c r="D73">
-        <v>103.72</v>
+        <v>120</v>
       </c>
       <c r="E73">
-        <f t="shared" si="3"/>
-        <v>135.09677605560398</v>
+        <f t="shared" si="14"/>
+        <v>148.14468184498614</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
-        <v>31.376776055603983</v>
+        <f t="shared" si="15"/>
+        <v>28.144681844986138</v>
       </c>
       <c r="G73">
-        <f t="shared" si="5"/>
-        <v>30.25142311569995</v>
+        <f t="shared" si="16"/>
+        <v>23.453901537488452</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2316,25 +2255,25 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C74">
-        <v>2.6669999999999998</v>
+        <v>2.82</v>
       </c>
       <c r="D74">
-        <v>104.68</v>
+        <v>120.83</v>
       </c>
       <c r="E74">
-        <f t="shared" si="3"/>
-        <v>135.99468967608576</v>
+        <f t="shared" si="14"/>
+        <v>150.9249413420371</v>
       </c>
       <c r="F74">
-        <f t="shared" si="4"/>
-        <v>31.314689676085749</v>
+        <f t="shared" si="15"/>
+        <v>30.094941342037103</v>
       </c>
       <c r="G74">
-        <f t="shared" si="5"/>
-        <v>29.914682533517144</v>
+        <f t="shared" si="16"/>
+        <v>24.906845437422078</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2342,29 +2281,543 @@
         <v>75</v>
       </c>
       <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75">
+        <v>2.7949999999999999</v>
+      </c>
+      <c r="D75">
+        <v>122.34</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="14"/>
+        <v>149.18489592068534</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="15"/>
+        <v>26.844895920685332</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="16"/>
+        <v>21.942860814684749</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <f>AVERAGE(C61:C75)</f>
+        <v>2.5198000000000005</v>
+      </c>
+      <c r="D76">
+        <f>AVERAGE(D61:D75)</f>
+        <v>107.16333333333333</v>
+      </c>
+      <c r="E76">
+        <f t="shared" ref="E76" si="17">AVERAGE(E61:E75)</f>
+        <v>130.79109681991335</v>
+      </c>
+      <c r="F76">
+        <f t="shared" ref="F76" si="18">AVERAGE(F61:F75)</f>
+        <v>23.627763486580026</v>
+      </c>
+      <c r="G76">
+        <f t="shared" ref="G76" si="19">AVERAGE(G61:G75)</f>
+        <v>22.421167180188878</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <f>STDEV(C61:C75)</f>
+        <v>0.20380179446847715</v>
+      </c>
+      <c r="D77">
+        <f>STDEV(D61:D75)</f>
+        <v>12.731296458876921</v>
+      </c>
+      <c r="E77">
+        <f>STDEV(E61:E75)</f>
+        <v>13.456029818674478</v>
+      </c>
+      <c r="F77">
+        <f>STDEV(F61:F75)</f>
+        <v>5.7497850780647157</v>
+      </c>
+      <c r="G77">
+        <f>STDEV(G61:G75)</f>
+        <v>6.025978866537554</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81">
+        <v>55</v>
+      </c>
+      <c r="B81">
         <v>40</v>
       </c>
-      <c r="C75">
+      <c r="C81">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="D81">
+        <v>72.040000000000006</v>
+      </c>
+      <c r="E81">
+        <f t="shared" ref="E81:E86" si="20">(C81*COS((PI()*B81/180))/-9.8)*(-C81*SIN(PI()*B81/180)-SQRT((C81*SIN(PI()*B81/180))^2-2*(-9.8)*(0.91+0.003*B81)))*100</f>
+        <v>102.53639567585282</v>
+      </c>
+      <c r="F81">
+        <f t="shared" ref="F81:F86" si="21">E81-D81</f>
+        <v>30.49639567585281</v>
+      </c>
+      <c r="G81">
+        <f t="shared" ref="G81:G86" si="22">(E81/D81-1)*100</f>
+        <v>42.332587001461434</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82">
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>40</v>
+      </c>
+      <c r="C82">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="D82">
+        <v>68.98</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="20"/>
+        <v>98.320186470314496</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="21"/>
+        <v>29.340186470314492</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="22"/>
+        <v>42.534338170940124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83">
+        <v>55</v>
+      </c>
+      <c r="B83">
+        <v>40</v>
+      </c>
+      <c r="C83">
+        <v>2.1429999999999998</v>
+      </c>
+      <c r="D83">
+        <v>71.11</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="20"/>
+        <v>101.79824621087627</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="21"/>
+        <v>30.688246210876272</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="22"/>
+        <v>43.156020546865804</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84">
+        <v>60</v>
+      </c>
+      <c r="B84">
+        <v>40</v>
+      </c>
+      <c r="C84">
+        <v>2.2509999999999999</v>
+      </c>
+      <c r="D84">
+        <v>80.540000000000006</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="20"/>
+        <v>108.51628936054276</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="21"/>
+        <v>27.976289360542751</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="22"/>
+        <v>34.735894413388067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85">
+        <v>60</v>
+      </c>
+      <c r="B85">
+        <v>40</v>
+      </c>
+      <c r="C85">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="D85">
+        <v>77.819999999999993</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="20"/>
+        <v>106.8835799183602</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="21"/>
+        <v>29.063579918360205</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="22"/>
+        <v>37.347185708507084</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86">
+        <v>60</v>
+      </c>
+      <c r="B86">
+        <v>40</v>
+      </c>
+      <c r="C86">
+        <v>2.2610000000000001</v>
+      </c>
+      <c r="D86">
+        <v>81.77</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="20"/>
+        <v>109.14686737844946</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="21"/>
+        <v>27.376867378449461</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="22"/>
+        <v>33.480331880212134</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87">
+        <v>65</v>
+      </c>
+      <c r="B87">
+        <v>40</v>
+      </c>
+      <c r="C87">
+        <v>2.3809999999999998</v>
+      </c>
+      <c r="D87">
+        <v>86.65</v>
+      </c>
+      <c r="E87">
+        <f t="shared" ref="E87:E95" si="23">(C87*COS((PI()*B87/180))/-9.8)*(-C87*SIN(PI()*B87/180)-SQRT((C87*SIN(PI()*B87/180))^2-2*(-9.8)*(0.91+0.003*B87)))*100</f>
+        <v>116.82770636493291</v>
+      </c>
+      <c r="F87">
+        <f t="shared" ref="F87:F95" si="24">E87-D87</f>
+        <v>30.177706364932902</v>
+      </c>
+      <c r="G87">
+        <f t="shared" ref="G87:G95" si="25">(E87/D87-1)*100</f>
+        <v>34.827127945681369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>65</v>
+      </c>
+      <c r="B88">
+        <v>40</v>
+      </c>
+      <c r="C88">
+        <v>2.415</v>
+      </c>
+      <c r="D88">
+        <v>89.38</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="23"/>
+        <v>119.04241182764423</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="24"/>
+        <v>29.662411827644235</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="25"/>
+        <v>33.186855927102535</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>65</v>
+      </c>
+      <c r="B89">
+        <v>40</v>
+      </c>
+      <c r="C89">
+        <v>2.371</v>
+      </c>
+      <c r="D89">
+        <v>85.38</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="23"/>
+        <v>116.17956827878793</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="24"/>
+        <v>30.79956827878793</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="25"/>
+        <v>36.073516372438434</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90">
+        <v>70</v>
+      </c>
+      <c r="B90">
+        <v>40</v>
+      </c>
+      <c r="C90">
+        <v>2.5529999999999999</v>
+      </c>
+      <c r="D90">
+        <v>94.74</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="23"/>
+        <v>128.20777790883764</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="24"/>
+        <v>33.467777908837647</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="25"/>
+        <v>35.325921373060631</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91">
+        <v>70</v>
+      </c>
+      <c r="B91">
+        <v>40</v>
+      </c>
+      <c r="C91">
+        <v>2.472</v>
+      </c>
+      <c r="D91">
+        <v>93.93</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="23"/>
+        <v>122.79370701846524</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="24"/>
+        <v>28.863707018465234</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="25"/>
+        <v>30.728954560273849</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92">
+        <v>70</v>
+      </c>
+      <c r="B92">
+        <v>40</v>
+      </c>
+      <c r="C92">
+        <v>2.536</v>
+      </c>
+      <c r="D92">
+        <v>96.5</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="23"/>
+        <v>127.06335008836211</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="24"/>
+        <v>30.563350088362114</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="25"/>
+        <v>31.671865376541053</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93">
+        <v>75</v>
+      </c>
+      <c r="B93">
+        <v>40</v>
+      </c>
+      <c r="C93">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="D93">
+        <v>103.72</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="23"/>
+        <v>135.09677605560398</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="24"/>
+        <v>31.376776055603983</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="25"/>
+        <v>30.25142311569995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94">
+        <v>75</v>
+      </c>
+      <c r="B94">
+        <v>40</v>
+      </c>
+      <c r="C94">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="D94">
+        <v>104.68</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="23"/>
+        <v>135.99468967608576</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="24"/>
+        <v>31.314689676085749</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="25"/>
+        <v>29.914682533517144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95">
+        <v>75</v>
+      </c>
+      <c r="B95">
+        <v>40</v>
+      </c>
+      <c r="C95">
         <v>2.6389999999999998</v>
       </c>
-      <c r="D75">
+      <c r="D95">
         <v>102.21</v>
       </c>
-      <c r="E75">
-        <f t="shared" si="3"/>
+      <c r="E95">
+        <f t="shared" si="23"/>
         <v>134.06390838048063</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="4"/>
+      <c r="F95">
+        <f t="shared" si="24"/>
         <v>31.853908380480632</v>
       </c>
-      <c r="G75">
-        <f t="shared" si="5"/>
+      <c r="G95">
+        <f t="shared" si="25"/>
         <v>31.165158380276516</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <f>AVERAGE(C81:C95)</f>
+        <v>2.3872666666666671</v>
+      </c>
+      <c r="D96">
+        <f>AVERAGE(D81:D95)</f>
+        <v>87.296666666666667</v>
+      </c>
+      <c r="E96">
+        <f t="shared" ref="E96" si="26">AVERAGE(E81:E95)</f>
+        <v>117.49809737423976</v>
+      </c>
+      <c r="F96">
+        <f t="shared" ref="F96" si="27">AVERAGE(F81:F95)</f>
+        <v>30.201430707573092</v>
+      </c>
+      <c r="G96">
+        <f t="shared" ref="G96" si="28">AVERAGE(G81:G95)</f>
+        <v>35.115457553731069</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97">
+        <f>STDEV(C81:C95)</f>
+        <v>0.19563576457527487</v>
+      </c>
+      <c r="D97">
+        <f>STDEV(D81:D95)</f>
+        <v>11.901769176211113</v>
+      </c>
+      <c r="E97">
+        <f>STDEV(E81:E95)</f>
+        <v>12.723109374340517</v>
+      </c>
+      <c r="F97">
+        <f>STDEV(F81:F95)</f>
+        <v>1.5556281117929693</v>
+      </c>
+      <c r="G97">
+        <f>STDEV(G81:G95)</f>
+        <v>4.4861056602000584</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>